<commit_message>
update excel and PDF
</commit_message>
<xml_diff>
--- a/metadata_template.xlsx
+++ b/metadata_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14235" tabRatio="913"/>
+    <workbookView xWindow="1860" yWindow="465" windowWidth="25605" windowHeight="14235" tabRatio="913" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="22" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="208">
   <si>
     <t>StorageType</t>
   </si>
@@ -619,6 +619,45 @@
   </si>
   <si>
     <t>Altitude Unit</t>
+  </si>
+  <si>
+    <t>https://utexas.box.com/v/ble-metadata-alaskaplacenames</t>
+  </si>
+  <si>
+    <t>Update Frequency</t>
+  </si>
+  <si>
+    <t>Update Frequencies</t>
+  </si>
+  <si>
+    <t>annually</t>
+  </si>
+  <si>
+    <t>asNeeded</t>
+  </si>
+  <si>
+    <t>biannually</t>
+  </si>
+  <si>
+    <t>continually</t>
+  </si>
+  <si>
+    <t>daily</t>
+  </si>
+  <si>
+    <t>irregular</t>
+  </si>
+  <si>
+    <t>monthly</t>
+  </si>
+  <si>
+    <t>notPlanned</t>
+  </si>
+  <si>
+    <t>weekly</t>
+  </si>
+  <si>
+    <t>unknown</t>
   </si>
 </sst>
 </file>
@@ -1233,7 +1272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1345,7 +1384,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:F23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1594,6 +1635,9 @@
         <v>41</v>
       </c>
       <c r="D13" s="1"/>
+      <c r="F13" s="15" t="s">
+        <v>197</v>
+      </c>
       <c r="I13" s="1" t="s">
         <v>24</v>
       </c>
@@ -1609,6 +1653,9 @@
         <v>101</v>
       </c>
       <c r="D14" s="1"/>
+      <c r="F14" t="s">
+        <v>198</v>
+      </c>
       <c r="I14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1621,6 +1668,9 @@
         <v>102</v>
       </c>
       <c r="D15" s="1"/>
+      <c r="F15" t="s">
+        <v>199</v>
+      </c>
       <c r="I15" s="1" t="s">
         <v>26</v>
       </c>
@@ -1631,6 +1681,9 @@
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="1"/>
+      <c r="F16" t="s">
+        <v>200</v>
+      </c>
       <c r="I16" s="1" t="s">
         <v>27</v>
       </c>
@@ -1641,12 +1694,18 @@
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="1"/>
+      <c r="F17" t="s">
+        <v>201</v>
+      </c>
       <c r="I17" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
+      <c r="F18" t="s">
+        <v>202</v>
+      </c>
       <c r="I18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1659,6 +1718,9 @@
       <c r="D19" s="24" t="s">
         <v>180</v>
       </c>
+      <c r="F19" t="s">
+        <v>203</v>
+      </c>
       <c r="I19" s="1" t="s">
         <v>29</v>
       </c>
@@ -1676,6 +1738,9 @@
       <c r="D20" s="1" t="s">
         <v>181</v>
       </c>
+      <c r="F20" t="s">
+        <v>204</v>
+      </c>
       <c r="I20" s="1" t="s">
         <v>2</v>
       </c>
@@ -1693,6 +1758,9 @@
       <c r="D21" s="1" t="s">
         <v>182</v>
       </c>
+      <c r="F21" t="s">
+        <v>205</v>
+      </c>
       <c r="I21" s="1" t="s">
         <v>12</v>
       </c>
@@ -1707,6 +1775,9 @@
       <c r="C22" s="6" t="s">
         <v>119</v>
       </c>
+      <c r="F22" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="23" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1717,6 +1788,9 @@
       </c>
       <c r="C23" s="6" t="s">
         <v>121</v>
+      </c>
+      <c r="F23" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1755,11 +1829,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,7 +1853,7 @@
     <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1822,8 +1896,11 @@
       <c r="N1" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F2"/>
       <c r="M2" t="s">
         <v>126</v>
@@ -1832,7 +1909,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -1854,7 +1931,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter a datum for the coordinates supplied in your dataset._x000a_" prompt="The datum for all coordinates in this dataset.  This is typically WGS_1984, especially if coordinates are from GPS. _x000a__x000a_Choose from a value in the drop down or enter your own value.">
           <x14:formula1>
             <xm:f>lookup_tables!$D$11:$D$12</xm:f>
@@ -1866,6 +1943,12 @@
             <xm:f>lookup_tables!$D$20:$D$21</xm:f>
           </x14:formula1>
           <xm:sqref>L2:L4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Will this data be ongoing?" prompt="And if so how often will it be updated? Choose from the drop-down. Note that frequency here is how often we upload new archival versions (e.g. most BLE core program data will be updated annually after the sampling season). ">
+          <x14:formula1>
+            <xm:f>lookup_tables!F14:F23</xm:f>
+          </x14:formula1>
+          <xm:sqref>O2:O4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1879,7 +1962,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1999,10 +2082,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2099,7 +2182,7 @@
         <v>77</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>78</v>
+        <v>195</v>
       </c>
       <c r="I5" s="32" t="s">
         <v>103</v>
@@ -2217,7 +2300,6 @@
     <hyperlink ref="H2" r:id="rId1"/>
     <hyperlink ref="H3" r:id="rId2"/>
     <hyperlink ref="H4" r:id="rId3"/>
-    <hyperlink ref="H5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2341,7 +2423,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Longitude in decimal degrees.  Longitudes west of the prime meridian are negative.  Use at least six decimal places." sqref="M2:M4">
       <formula1>-180</formula1>
       <formula2>180</formula2>
@@ -2350,6 +2432,7 @@
       <formula1>-90</formula1>
       <formula2>90</formula2>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="For core program datasets: put a list of CP stations appearing in the data. No need to put in coords, except if there are sites not listed here https://utexas.box.com/v/ble-coreprogram-stations, for example if an ocean site that changes every year" sqref="D2:D4"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2361,7 +2444,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2600,7 +2683,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2680,7 +2763,7 @@
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update title, abstract, and attribute desc word count guides for FAIR
</commit_message>
<xml_diff>
--- a/metadata_template.xlsx
+++ b/metadata_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\austin.utexas.edu\disk\engr\research\crwr\Projects\BLE-LTER\Data-Notes\BLE-Practices\metadata_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Data-Notes\BLE-Practices\metadata_templates\canon\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="465" windowWidth="25605" windowHeight="14235" tabRatio="913" activeTab="3"/>
+    <workbookView xWindow="3300" yWindow="465" windowWidth="25605" windowHeight="14235" tabRatio="913" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="22" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="210">
   <si>
     <t>StorageType</t>
   </si>
@@ -658,6 +658,12 @@
   </si>
   <si>
     <t>unknown</t>
+  </si>
+  <si>
+    <t>Core Program?</t>
+  </si>
+  <si>
+    <t>Primary funded by BLE LTER?</t>
   </si>
 </sst>
 </file>
@@ -1829,11 +1835,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomLeft" activeCell="P2" sqref="P2:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1841,19 +1847,22 @@
     <col min="1" max="1" width="9.28515625" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="8.140625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="37" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" style="2" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" customWidth="1"/>
+    <col min="16" max="16" width="14" customWidth="1"/>
+    <col min="17" max="17" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1899,8 +1908,14 @@
       <c r="O1" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F2"/>
       <c r="M2" t="s">
         <v>126</v>
@@ -1909,7 +1924,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -1920,7 +1935,7 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ideally less than 15 words. What (theme+taxa), where, when, and also who and why if there's room, e.g.,_x000a__x000a_Carbon flux from aquatic ecosystems of the Arctic Coastal Plain along the Beaufort Sea, Alaska, from 2010-2018" sqref="D2:D4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ideally less than 20 words. What (theme+taxa), where, when, and also who and why if there's room, e.g.,_x000a__x000a_Carbon flux from aquatic ecosystems of the Arctic Coastal Plain along the Beaufort Sea, Alaska, from 2010-2018" sqref="D2:D4"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Send us a Word doc and enter file name here. See PDF for guidelines." sqref="E2:E4 H2:H4"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Earliest date in dataset. Use YYYY-MM-DD or YYYY." sqref="I2:I4"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latest date in dataset. Use YYYY-MM-DD or YYYY." sqref="J2:J4"/>
@@ -2082,7 +2097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
@@ -2341,7 +2356,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Change "primary" to "primarily" and add some input messages
</commit_message>
<xml_diff>
--- a/metadata_template.xlsx
+++ b/metadata_template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\austin.utexas.edu\disk\engr\research\crwr\Projects\BLE-LTER\Data-Notes\BLE-Practices\metadata_templates\canon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whiteatl\Documents\ble-metadata-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EB50C2-4FE8-4CCB-98D0-F9706D5FEF95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="468" windowWidth="24060" windowHeight="12552" tabRatio="913" activeTab="11"/>
+    <workbookView xWindow="6180" yWindow="465" windowWidth="24060" windowHeight="12555" tabRatio="913" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="22" r:id="rId1"/>
@@ -25,7 +26,7 @@
     <sheet name="Taxonomic" sheetId="26" state="hidden" r:id="rId11"/>
     <sheet name="lookup_tables" sheetId="24" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -664,9 +665,6 @@
     <t>Core Program?</t>
   </si>
   <si>
-    <t>Primary funded by BLE LTER?</t>
-  </si>
-  <si>
     <t>Relationship to Dataset</t>
   </si>
   <si>
@@ -683,12 +681,15 @@
   </si>
   <si>
     <t>data cites pub (method/idea)</t>
+  </si>
+  <si>
+    <t>Primarily funded by BLE LTER?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -1017,7 +1018,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1294,16 +1295,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27"/>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -1318,7 +1317,7 @@
       <c r="L1" s="27"/>
       <c r="M1" s="27"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27"/>
       <c r="B2" s="27" t="s">
         <v>132</v>
@@ -1335,7 +1334,7 @@
       <c r="L2" s="27"/>
       <c r="M2" s="27"/>
     </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
       <c r="B3" s="27" t="s">
         <v>186</v>
@@ -1352,7 +1351,7 @@
       <c r="L3" s="27"/>
       <c r="M3" s="27"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
@@ -1374,185 +1373,190 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="indicate the relationship between the dataset and the publication" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="info to ID the publication: can be a citation (any format), a DOI, a link" sqref="A1"/>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="info to ID the publication: can be a citation (any format), a DOI, a link" sqref="A2" xr:uid="{00000000-0002-0000-0900-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000002000000}">
           <x14:formula1>
             <xm:f>lookup_tables!A$28:A$30</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B50</xm:sqref>
+          <xm:sqref>B3:B50</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="indicate the relationship between the dataset and the publication" xr:uid="{9E8765E9-F65F-464B-95B5-1696289C937F}">
+          <x14:formula1>
+            <xm:f>lookup_tables!A$28:A$30</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1561,21 +1565,21 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>127</v>
       </c>
@@ -1595,25 +1599,23 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:A30"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="2" max="2" width="41.5546875" customWidth="1"/>
-    <col min="3" max="3" width="31.88671875" customWidth="1"/>
-    <col min="4" max="4" width="44.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="64.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="41.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" customWidth="1"/>
+    <col min="4" max="4" width="44.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="64.5703125" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>86</v>
       </c>
@@ -1628,7 +1630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>54</v>
       </c>
@@ -1651,7 +1653,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>72</v>
       </c>
@@ -1674,7 +1676,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>57</v>
       </c>
@@ -1694,7 +1696,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>59</v>
       </c>
@@ -1714,7 +1716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>77</v>
       </c>
@@ -1737,7 +1739,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>79</v>
       </c>
@@ -1755,7 +1757,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>82</v>
       </c>
@@ -1773,7 +1775,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F9" s="14" t="s">
         <v>94</v>
       </c>
@@ -1781,7 +1783,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>87</v>
       </c>
@@ -1804,7 +1806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1821,7 +1823,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -1838,7 +1840,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1856,7 +1858,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -1874,7 +1876,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
         <v>30</v>
       </c>
@@ -1889,7 +1891,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
         <v>31</v>
       </c>
@@ -1902,7 +1904,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
         <v>6</v>
       </c>
@@ -1915,7 +1917,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
       <c r="F18" t="s">
         <v>202</v>
@@ -1924,7 +1926,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>104</v>
       </c>
@@ -1939,7 +1941,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>105</v>
       </c>
@@ -1959,7 +1961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>108</v>
       </c>
@@ -1979,7 +1981,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>109</v>
       </c>
@@ -1993,7 +1995,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>110</v>
       </c>
@@ -2007,7 +2009,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -2018,7 +2020,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>112</v>
       </c>
@@ -2029,33 +2031,33 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>211</v>
       </c>
-      <c r="B27" s="4"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>212</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>213</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C4" r:id="rId2"/>
-    <hyperlink ref="C5" r:id="rId3"/>
-    <hyperlink ref="C6" r:id="rId4"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{00000000-0004-0000-0B00-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -2063,35 +2065,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K26" sqref="K26"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.88671875" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" customWidth="1"/>
     <col min="16" max="16" width="14" customWidth="1"/>
-    <col min="17" max="17" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -2141,10 +2143,10 @@
         <v>208</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F2"/>
       <c r="M2" t="s">
         <v>126</v>
@@ -2152,8 +2154,9 @@
       <c r="N2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -2163,32 +2166,38 @@
       <c r="N4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ideally less than 20 words. What (theme+taxa), where, when, and also who and why if there's room, e.g.,_x000a__x000a_Carbon flux from aquatic ecosystems of the Arctic Coastal Plain along the Beaufort Sea, Alaska, from 2010-2018" sqref="D2:D4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Send us a Word doc and enter file name here. See PDF for guidelines." sqref="E2:E4 H2:H4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Earliest date in dataset. Use YYYY-MM-DD or YYYY." sqref="I2:I4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latest date in dataset. Use YYYY-MM-DD or YYYY." sqref="J2:J4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="CC0 or Creative Commons 0, a public domain license, is the license we use for our datasets. If you wish to use a different license, please discuss with the information managers." sqref="M2:M4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The timezone used for any date/time values supplied in this dataset." sqref="N2:N4"/>
+  <dataValidations count="8">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ideally less than 20 words. What (theme+taxa), where, when, and also who and why if there's room, e.g.,_x000a__x000a_Carbon flux from aquatic ecosystems of the Arctic Coastal Plain along the Beaufort Sea, Alaska, from 2010-2018" sqref="D2:D4" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Send us a Word doc and enter file name here. See PDF for guidelines." sqref="E2:E4 H2:H4" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Earliest date in dataset. Use YYYY-MM-DD or YYYY." sqref="I2:I4" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latest date in dataset. Use YYYY-MM-DD or YYYY." sqref="J2:J4" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="CC0 or Creative Commons 0, a public domain license, is the license we use for our datasets. If you wish to use a different license, please discuss with the information managers." sqref="M2:M4" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The timezone used for any date/time values supplied in this dataset." sqref="N2:N4" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Was this dataset primarly funded by BLE? If not, you'll need to provide the information manager with details about other projects funding this dataset." sqref="Q2" xr:uid="{BF42C68D-2709-4EEF-BD9A-D102563989B3}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Is this a BLE Core Program dataset?" sqref="P2" xr:uid="{D3AF8956-7671-4D19-B1E6-17F41F8A5B56}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter a datum for the coordinates supplied in your dataset._x000a_" prompt="The datum for all coordinates in this dataset.  This is typically WGS_1984, especially if coordinates are from GPS. _x000a__x000a_Choose from a value in the drop down or enter your own value.">
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter a datum for the coordinates supplied in your dataset._x000a_" prompt="The datum for all coordinates in this dataset.  This is typically WGS_1984, especially if coordinates are from GPS. _x000a__x000a_Choose from a value in the drop down or enter your own value." xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$D$11:$D$12</xm:f>
           </x14:formula1>
           <xm:sqref>K2:K4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="make sure we can locate this authority" prompt="The taxonomic authority to which you refer when determining taxonomic names in this dataset. The drop-down options are ITIS and WoRMS, commonly used in marine bio, or enter your own.">
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="make sure we can locate this authority" prompt="The taxonomic authority to which you refer when determining taxonomic names in this dataset. The drop-down options are ITIS and WoRMS, commonly used in marine bio, or enter your own." xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$D$20:$D$21</xm:f>
           </x14:formula1>
           <xm:sqref>L2:L4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Will this data be ongoing?" prompt="And if so how often will it be updated? Choose from the drop-down. Note that frequency here is how often we upload new archival versions (e.g. most BLE core program data will be updated annually after the sampling season). ">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Will this data be ongoing?" prompt="And if so how often will it be updated? Choose from the drop-down. Note that frequency here is how often we upload new archival versions (e.g. most BLE core program data will be updated annually after the sampling season). " xr:uid="{00000000-0002-0000-0100-000008000000}">
           <x14:formula1>
             <xm:f>lookup_tables!F14:F23</xm:f>
           </x14:formula1>
@@ -2201,32 +2210,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R2" sqref="R2"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="1"/>
-    <col min="8" max="8" width="14.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" style="1" customWidth="1"/>
-    <col min="10" max="15" width="8.88671875" style="1"/>
-    <col min="16" max="16" width="8.88671875" style="3"/>
-    <col min="17" max="17" width="21.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="13.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="14.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="1" customWidth="1"/>
+    <col min="10" max="15" width="8.85546875" style="1"/>
+    <col min="16" max="16" width="8.85546875" style="3"/>
+    <col min="17" max="17" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
@@ -2293,24 +2302,24 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="let us know if you think this custom role needs to be in our semi-controlled list" sqref="C1"/>
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Number all creators starting with 2." prompt="Analogous to authorship order in a publication. Per LTER best practices, BLE will be first creator to any BLE dataset, so number all creators starting with 2. _x000a__x000a_Leave blank for all other roles." sqref="D2:D4">
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="let us know if you think this custom role needs to be in our semi-controlled list" sqref="C1" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Number all creators starting with 2." prompt="Analogous to authorship order in a publication. Per LTER best practices, BLE will be first creator to any BLE dataset, so number all creators starting with 2. _x000a__x000a_Leave blank for all other roles." sqref="D2:D4" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>2</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="ORCID is a unique identifier system for researchers. Sign up at https://orcid.org. This person doesn't have an ORCID? Maybe encourage them to get one and fill out a profile? (Merely having an ORCID is no good without a nice profile.)" sqref="H2:H4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="ORCID is a unique identifier system for researchers. Sign up at https://orcid.org. This person doesn't have an ORCID? Maybe encourage them to get one and fill out a profile? (Merely having an ORCID is no good without a nice profile.)" sqref="H2:H4" xr:uid="{00000000-0002-0000-0200-000002000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="let us know if you think this custom role needs to be in our semi-controlled list">
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="let us know if you think this custom role needs to be in our semi-controlled list" xr:uid="{00000000-0002-0000-0200-000003000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$F$3:$F$10</xm:f>
           </x14:formula1>
           <xm:sqref>C5:C1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" prompt="Include dataset creators, but also technicians and other personnel who contribute to and deserve acknowledgment for this dataset._x000a__x000a_Choose from a value in the drop down or enter your own value.">
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" prompt="Include dataset creators, but also technicians and other personnel who contribute to and deserve acknowledgment for this dataset._x000a__x000a_Choose from a value in the drop down or enter your own value." xr:uid="{00000000-0002-0000-0200-000004000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$F$3:$F$10</xm:f>
           </x14:formula1>
@@ -2323,30 +2332,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="6" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" style="6" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5546875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="6" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="6" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="6" customWidth="1"/>
     <col min="7" max="7" width="40" style="6" customWidth="1"/>
-    <col min="8" max="8" width="36.6640625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="80.33203125" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="8" max="8" width="36.7109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="80.28515625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
@@ -2372,7 +2381,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D2" s="6" t="e">
         <f>VLOOKUP(C2, lookup_tables!$A$3:$B$8, 2, FALSE)</f>
         <v>#N/A</v>
@@ -2387,7 +2396,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D3" s="6" t="e">
         <f>VLOOKUP(C3, lookup_tables!$A$3:$B$8, 2, FALSE)</f>
         <v>#N/A</v>
@@ -2402,7 +2411,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D4" s="6" t="e">
         <f>VLOOKUP(C4, lookup_tables!$A$3:$B$8, 2, FALSE)</f>
         <v>#N/A</v>
@@ -2417,7 +2426,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D5" s="6" t="e">
         <f>VLOOKUP(C5, lookup_tables!$A$3:$B$8, 2, FALSE)</f>
         <v>#N/A</v>
@@ -2432,7 +2441,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D6" s="6" t="e">
         <f>VLOOKUP(C6, lookup_tables!$A$3:$B$8, 2, FALSE)</f>
         <v>#N/A</v>
@@ -2445,7 +2454,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="6" t="e">
         <f>VLOOKUP(C7, lookup_tables!$A$3:$B$8, 2, FALSE)</f>
         <v>#N/A</v>
@@ -2458,79 +2467,79 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D8" s="6" t="e">
         <f>VLOOKUP(C8, lookup_tables!$A$3:$B$8, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D9" s="6" t="e">
         <f>VLOOKUP(C9, lookup_tables!$A$3:$B$8, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D10" s="6" t="e">
         <f>VLOOKUP(C10, lookup_tables!$A$3:$B$8, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D11" s="6" t="e">
         <f>VLOOKUP(C11, lookup_tables!$A$3:$B$8, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D12" s="6" t="e">
         <f>VLOOKUP(C12, lookup_tables!$A$3:$B$8, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D13" s="6" t="e">
         <f>VLOOKUP(C13, lookup_tables!$A$3:$B$8, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14" s="6" t="e">
         <f>VLOOKUP(C14, lookup_tables!$A$3:$B$8, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D15" s="6" t="e">
         <f>VLOOKUP(C15, lookup_tables!$A$3:$B$8, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D16" s="6" t="e">
         <f>VLOOKUP(C16, lookup_tables!$A$3:$B$8, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="6" t="e">
         <f>VLOOKUP(C17, lookup_tables!$A$3:$B$8, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="6" t="e">
         <f>VLOOKUP(C18, lookup_tables!$A$3:$B$8, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="6" t="e">
         <f>VLOOKUP(C19, lookup_tables!$A$3:$B$8, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="6" t="e">
         <f>VLOOKUP(C20, lookup_tables!$A$3:$B$8, 2, FALSE)</f>
         <v>#N/A</v>
@@ -2538,36 +2547,36 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Keywords aid data discovery and context. You might want to re-use keywords in related publications, but make sure to find them in a thesaurus." sqref="B2:B4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Keywords aid data discovery and context. You might want to re-use keywords in related publications, but make sure to find them in a thesaurus." sqref="B2:B4" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2"/>
-    <hyperlink ref="H4" r:id="rId3"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="no custom value allowed here, I'm afraid">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="no custom value allowed here, I'm afraid" xr:uid="{00000000-0002-0000-0300-000001000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$C$11:$C$15</xm:f>
           </x14:formula1>
           <xm:sqref>E5:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000002000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$A$3:$A$8</xm:f>
           </x14:formula1>
           <xm:sqref>C5:C1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="We highly recommend choosing keywords from an existing keyword set, aka thesaurus. See the included table for links to preferred thesauri. _x000a__x000a_Choose from the drop-down menu. Choose &quot;none&quot; if the keyword did not come from any thesauri (not recommended!).">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="We highly recommend choosing keywords from an existing keyword set, aka thesaurus. See the included table for links to preferred thesauri. _x000a__x000a_Choose from the drop-down menu. Choose &quot;none&quot; if the keyword did not come from any thesauri (not recommended!)." xr:uid="{00000000-0002-0000-0300-000003000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$A$3:$A$8</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="no custom value allowed here, I'm afraid" prompt="Choose from the drop-down menu the keyword type applicable to this keyword.">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="no custom value allowed here, I'm afraid" prompt="Choose from the drop-down menu the keyword type applicable to this keyword." xr:uid="{00000000-0002-0000-0300-000004000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$C$11:$C$15</xm:f>
           </x14:formula1>
@@ -2580,35 +2589,35 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N1" sqref="N1"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="23.6640625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="23.109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="24.44140625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="24.33203125" hidden="1" customWidth="1"/>
-    <col min="13" max="14" width="24.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.6640625" customWidth="1"/>
-    <col min="16" max="16" width="12.88671875" customWidth="1"/>
-    <col min="17" max="17" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="24.28515625" hidden="1" customWidth="1"/>
+    <col min="13" max="14" width="24.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -2661,51 +2670,51 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>131</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Longitude in decimal degrees.  Longitudes west of the prime meridian are negative.  Use at least six decimal places." sqref="M2:M4">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Longitude in decimal degrees.  Longitudes west of the prime meridian are negative.  Use at least six decimal places." sqref="M2:M4" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>-180</formula1>
       <formula2>180</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latitude in decimal degrees.  Latitudes south of the equator are negative.  Use at least six decimal places." sqref="N2:N4">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latitude in decimal degrees.  Latitudes south of the equator are negative.  Use at least six decimal places." sqref="N2:N4" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>-90</formula1>
       <formula2>90</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="For core program datasets: put a list of CP stations appearing in the data. No need to put in coords, except if there are sites not listed here https://utexas.box.com/v/ble-coreprogram-stations, for example if an ocean site that changes every year" sqref="D2:D4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="For core program datasets: put a list of CP stations appearing in the data. No need to put in coords, except if there are sites not listed here https://utexas.box.com/v/ble-coreprogram-stations, for example if an ocean site that changes every year" sqref="D2:D4" xr:uid="{00000000-0002-0000-0400-000002000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="1" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="24.109375" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="34.88671875" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="1" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="8" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="21.88671875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="8.109375" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="49.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -2737,66 +2746,66 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2"/>
       <c r="D2"/>
       <c r="F2"/>
       <c r="I2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3"/>
       <c r="C3" s="1"/>
       <c r="D3"/>
       <c r="F3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B1048576" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Describe the data in this entity in two sentences or less. Situate this data within the larger dataset." sqref="E2:E4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Human-friendly name for this entity. Seven words or less, e.g., &quot;Elson plant community survey 2016&quot;. We might edit for clarity and brevity." sqref="C2:C4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Describe the data in this entity in two sentences or less. Situate this data within the larger dataset." sqref="E2:E4" xr:uid="{00000000-0002-0000-0500-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Human-friendly name for this entity. Seven words or less, e.g., &quot;Elson plant community survey 2016&quot;. We might edit for clarity and brevity." sqref="C2:C4" xr:uid="{00000000-0002-0000-0500-000002000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="23.109375" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="33.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="27.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="17.88671875" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="20.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" style="1" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="1"/>
+    <col min="17" max="17" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
@@ -2850,33 +2859,27 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="12">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="please enter whole numbers numbering your columns" sqref="C101:C1048576">
+  <dataValidations count="10">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="please enter whole numbers numbering your columns" sqref="C101:C1048576" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter whole numbers to number your columns starting from 1." sqref="C5:C25 C29:C100">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter whole numbers to number your columns starting from 1." sqref="C5:C100" xr:uid="{00000000-0002-0000-0600-000001000000}">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a numeric value &gt;= 0 for precision." sqref="N29:N43 N45:N100 N5:N25">
+    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a numeric value &gt;= 0 for precision." sqref="N45:N100 N5:N43" xr:uid="{00000000-0002-0000-0600-000002000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a numeric value." sqref="P2:Q100">
+    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a numeric value." sqref="P2:Q100" xr:uid="{00000000-0002-0000-0600-000003000000}">
       <formula1>ISNUMBER(P1)</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter whole numbers to number your columns starting from 1." prompt="Within each data table, number the columns from left, starting from 1. " sqref="C2:C4">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter whole numbers to number your columns starting from 1." prompt="Within each data table, number the columns from left, starting from 1. " sqref="C2:C4" xr:uid="{00000000-0002-0000-0600-000004000000}">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The exact column name as it appears in the data. _x000a__x000a_Good column names: informative, no spaces, no special characters, not starting with a number, ideally as few characters as possible without sacrificing information." sqref="D2:D4"/>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter whole numbers to number your columns starting from 1." sqref="C26:C28">
-      <formula1>1</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a numeric value &gt;= 0 for precision." sqref="N26:N28">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid entity" error="Please enter an entity number you have entered on the &quot;entities&quot; sheet" sqref="B101:B1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Make the information contained in this column as unambigous as possible. Spell out acronyms here. Spell out chemical speciation here. " sqref="G2:G4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If the attribute carries a unit, specify it here. Beware of coefficients; they often have units too. Put down &quot;dimensionless&quot; for counts or &quot;percent&quot; for percentages." sqref="M2:M4"/>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a numeric value &gt;= 0 for precision." prompt="Specify if attribute is numeric; leave blank otherwise. Specify the smallest unit at which you are confident in the data. E.g., 0.01 if data in this column go to two decimal places." sqref="N2:N4">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The exact column name as it appears in the data. _x000a__x000a_Good column names: informative, no spaces, no special characters, not starting with a number, ideally as few characters as possible without sacrificing information." sqref="D2:D4" xr:uid="{00000000-0002-0000-0600-000005000000}"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid entity" error="Please enter an entity number you have entered on the &quot;entities&quot; sheet" sqref="B101:B1048576" xr:uid="{00000000-0002-0000-0600-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Make the information contained in this column as unambigous as possible. Spell out acronyms here. Spell out chemical speciation here. " sqref="G2:G4" xr:uid="{00000000-0002-0000-0600-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If the attribute carries a unit, specify it here. Beware of coefficients; they often have units too. Put down &quot;dimensionless&quot; for counts or &quot;percent&quot; for percentages." sqref="M2:M4" xr:uid="{00000000-0002-0000-0600-00000A000000}"/>
+    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter a numeric value &gt;= 0 for precision." prompt="Specify if attribute is numeric; leave blank otherwise. Specify the smallest unit at which you are confident in the data. E.g., 0.01 if data in this column go to two decimal places." sqref="N2:N4" xr:uid="{00000000-0002-0000-0600-00000B000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -2885,31 +2888,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from the four!" prompt="choose from four number types">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from the four!" prompt="choose from four number types" xr:uid="{00000000-0002-0000-0600-00000C000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$A$11:$A$14</xm:f>
           </x14:formula1>
           <xm:sqref>O2:O1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not an option" error="choose from the seven!" prompt="choose from the seven">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not an option" error="choose from the seven!" prompt="choose from the seven" xr:uid="{00000000-0002-0000-0600-00000D000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$B$11:$B$17</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I24 I29:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not an option">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not an option" xr:uid="{00000000-0002-0000-0600-00000E000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$I$2:$I$21</xm:f>
           </x14:formula1>
           <xm:sqref>H2:H24 H29:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid entity" error="Please enter a file or worksheet name that appears on the &quot;entities&quot; sheet" prompt="Where does this column/attribute appear? The drop-down options correspond to entries in the &quot;Entities&quot; sheet.">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid entity" error="Please enter a file or worksheet name that appears on the &quot;entities&quot; sheet" prompt="Where does this column/attribute appear? The drop-down options correspond to entries in the &quot;Entities&quot; sheet." xr:uid="{00000000-0002-0000-0600-00000F000000}">
           <x14:formula1>
             <xm:f>Entities!$C$2:$C$30</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid entity" error="Please enter an entity number you have entered on the &quot;entities&quot; sheet">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid entity" error="Please enter an entity number you have entered on the &quot;entities&quot; sheet" xr:uid="{00000000-0002-0000-0600-000010000000}">
           <x14:formula1>
             <xm:f>Entities!$C$2:$C$30</xm:f>
           </x14:formula1>
@@ -2922,23 +2925,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="69" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -2955,40 +2958,40 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Exact code as appears in data." sqref="D2:D4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Define this code (even if it seems self-explanatory)." sqref="E2:E4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Exact code as appears in data." sqref="D2:D4" xr:uid="{00000000-0002-0000-0700-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Define this code (even if it seems self-explanatory)." sqref="E2:E4" xr:uid="{00000000-0002-0000-0700-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name that you have entered in the &quot;Attributes&quot; sheet">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name that you have entered in the &quot;Attributes&quot; sheet" xr:uid="{00000000-0002-0000-0700-000002000000}">
           <x14:formula1>
             <xm:f>Attributes!$D:$D</xm:f>
           </x14:formula1>
           <xm:sqref>C5:C1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid entity" error="Please enter a file or worksheet name that appears on the &quot;entities&quot; sheet" prompt="Where does this column/attribute appear? The drop-down options correspond to entries in the &quot;Entities&quot; sheet.">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid entity" error="Please enter a file or worksheet name that appears on the &quot;entities&quot; sheet" prompt="Where does this column/attribute appear? The drop-down options correspond to entries in the &quot;Entities&quot; sheet." xr:uid="{00000000-0002-0000-0700-000003000000}">
           <x14:formula1>
             <xm:f>Entities!$C$2:$C$30</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid entity" error="Please enter an entity number you have entered on the &quot;entities&quot; sheet">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid entity" error="Please enter an entity number you have entered on the &quot;entities&quot; sheet" xr:uid="{00000000-0002-0000-0700-000004000000}">
           <x14:formula1>
             <xm:f>Entities!$B$2:$B$30</xm:f>
           </x14:formula1>
           <xm:sqref>B5:B1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name that appears in the &quot;Attributes&quot; sheet" prompt="Where does this code appear? The drop-down options correspond to entries in &quot;Attributes&quot; sheet.">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name that appears in the &quot;Attributes&quot; sheet" prompt="Where does this code appear? The drop-down options correspond to entries in &quot;Attributes&quot; sheet." xr:uid="{00000000-0002-0000-0700-000005000000}">
           <x14:formula1>
             <xm:f>Attributes!$D:$D</xm:f>
           </x14:formula1>
@@ -3001,25 +3004,25 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -3036,42 +3039,42 @@
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="E4" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Exact missing value code as appears in data." sqref="D2:D4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Reason for missing value." sqref="E2:E4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Exact missing value code as appears in data." sqref="D2:D4" xr:uid="{00000000-0002-0000-0800-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Reason for missing value." sqref="E2:E4" xr:uid="{00000000-0002-0000-0800-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid entity" error="Please enter an entity number you have entered on the &quot;entities&quot; sheet">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid entity" error="Please enter an entity number you have entered on the &quot;entities&quot; sheet" xr:uid="{00000000-0002-0000-0800-000002000000}">
           <x14:formula1>
             <xm:f>Entities!$B$2:$B$30</xm:f>
           </x14:formula1>
           <xm:sqref>B5:B1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name you have entered in the &quot;attributes&quot; sheet">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name you have entered in the &quot;attributes&quot; sheet" xr:uid="{00000000-0002-0000-0800-000003000000}">
           <x14:formula1>
             <xm:f>Attributes!$D:$D</xm:f>
           </x14:formula1>
           <xm:sqref>C5:C1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid entity" error="Please enter a file or worksheet name that appears on the &quot;entities&quot; sheet" prompt="Where does this column/attribute appear? The drop-down options correspond to entries in the &quot;Entities&quot; sheet.">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid entity" error="Please enter a file or worksheet name that appears on the &quot;entities&quot; sheet" prompt="Where does this column/attribute appear? The drop-down options correspond to entries in the &quot;Entities&quot; sheet." xr:uid="{00000000-0002-0000-0800-000004000000}">
           <x14:formula1>
             <xm:f>Entities!$C$2:$C$30</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name that appears on the &quot;attributes&quot; sheet" prompt="Where does this code appear? The drop-down options correspond to entries in &quot;Attributes&quot; sheet.">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid column name" error="Please enter a column name that appears on the &quot;attributes&quot; sheet" prompt="Where does this code appear? The drop-down options correspond to entries in &quot;Attributes&quot; sheet." xr:uid="{00000000-0002-0000-0800-000005000000}">
           <x14:formula1>
             <xm:f>Attributes!$D:$D</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Better describe what Core Program means in Excel input message
</commit_message>
<xml_diff>
--- a/metadata_template.xlsx
+++ b/metadata_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whiteatl\Documents\ble-metadata-template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\austin.utexas.edu\disk\engr\research\crwr\Projects\BLE-LTER\Data-Notes\BLE-Practices\metadata_templates\canon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EB50C2-4FE8-4CCB-98D0-F9706D5FEF95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559EAA8B-8CA8-4230-970C-A268AB5D22A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="465" windowWidth="24060" windowHeight="12555" tabRatio="913" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6180" yWindow="465" windowWidth="24060" windowHeight="12555" tabRatio="913" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="22" r:id="rId1"/>
@@ -1298,7 +1298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2068,7 +2068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
@@ -2176,7 +2176,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Was this dataset primarly funded by BLE? If not, you'll need to provide the information manager with details about other projects funding this dataset." sqref="Q2" xr:uid="{BF42C68D-2709-4EEF-BD9A-D102563989B3}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Is this a BLE Core Program dataset?" sqref="P2" xr:uid="{D3AF8956-7671-4D19-B1E6-17F41F8A5B56}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Is this a BLE Core Program dataset? This does NOT necessarily refer to ice or soil cores, but whether this is a dataset that BLE commits to updating each year (&quot;core&quot; as in central or foundational). If you don't know, then the answer is probably No." sqref="P2" xr:uid="{D3AF8956-7671-4D19-B1E6-17F41F8A5B56}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2184,7 +2184,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter a datum for the coordinates supplied in your dataset._x000a_" prompt="The datum for all coordinates in this dataset.  This is typically WGS_1984, especially if coordinates are from GPS. _x000a__x000a_Choose from a value in the drop down or enter your own value." xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>lookup_tables!$D$11:$D$12</xm:f>
@@ -2199,9 +2199,15 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Will this data be ongoing?" prompt="And if so how often will it be updated? Choose from the drop-down. Note that frequency here is how often we upload new archival versions (e.g. most BLE core program data will be updated annually after the sampling season). " xr:uid="{00000000-0002-0000-0100-000008000000}">
           <x14:formula1>
+            <xm:f>lookup_tables!F15:F24</xm:f>
+          </x14:formula1>
+          <xm:sqref>O3:O4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Will this data be ongoing?" prompt="And if so how often will it be updated? Choose from the drop-down. Note that frequency here is how often we upload new archival versions (e.g., most BLE core program data will be updated annually after the sampling season). " xr:uid="{2051BC9A-15C4-49F9-8E20-717C0D8FE730}">
+          <x14:formula1>
             <xm:f>lookup_tables!F14:F23</xm:f>
           </x14:formula1>
-          <xm:sqref>O2:O4</xm:sqref>
+          <xm:sqref>O2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>